<commit_message>
update New Function Skip Inference
</commit_message>
<xml_diff>
--- a/temp_files/历代配种方案及出雏对照2021_带性别.xlsx
+++ b/temp_files/历代配种方案及出雏对照2021_带性别.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19930" windowHeight="16790" activeTab="3"/>
+    <workbookView windowWidth="15620" windowHeight="12450" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="16" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="18" sheetId="5" r:id="rId3"/>
     <sheet name="19" sheetId="6" r:id="rId4"/>
     <sheet name="20" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -14632,7 +14631,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -20915,8 +20914,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -24702,20 +24701,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>